<commit_message>
adding more RFU data
</commit_message>
<xml_diff>
--- a/data-general/chlamy-population-key.xlsx
+++ b/data-general/chlamy-population-key.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Number</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>CC-1690</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
@@ -506,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -533,8 +539,14 @@
       <c r="F1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -550,8 +562,14 @@
       <c r="E2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>39.045752999999998</v>
+      </c>
+      <c r="H2">
+        <v>-76.641272999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8</v>
       </c>
@@ -567,8 +585,14 @@
       <c r="E3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>42.375801000000003</v>
+      </c>
+      <c r="H3">
+        <v>-72.519867000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -581,8 +605,14 @@
       <c r="E4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>27.664826999999999</v>
+      </c>
+      <c r="H4">
+        <v>-81.515754999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -596,7 +626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -613,7 +643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -629,8 +659,14 @@
       <c r="E7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>46.227637999999999</v>
+      </c>
+      <c r="H7">
+        <v>2.213749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
@@ -646,8 +682,14 @@
       <c r="E8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>35.759574999999998</v>
+      </c>
+      <c r="H8">
+        <v>-79.019301999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>11</v>
       </c>
@@ -663,8 +705,14 @@
       <c r="E9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>39.550052999999998</v>
+      </c>
+      <c r="H9">
+        <v>-105.782066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -680,8 +728,14 @@
       <c r="E10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>42.477150000000002</v>
+      </c>
+      <c r="H10">
+        <v>-72.607950000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -697,8 +751,14 @@
       <c r="E11" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>42.375801000000003</v>
+      </c>
+      <c r="H11">
+        <v>-72.519867000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
@@ -715,7 +775,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -735,7 +795,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -749,13 +809,19 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>42.375801000000003</v>
+      </c>
+      <c r="H14">
+        <v>-72.519867000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
@@ -775,7 +841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>

</xml_diff>